<commit_message>
Code updates to automate table compiling depending on file type.
</commit_message>
<xml_diff>
--- a/External_data/FlowScen/FallFlows20240909_Draft.xlsx
+++ b/External_data/FlowScen/FallFlows20240909_Draft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/ebuttermore_usbr_gov/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cehlo_usbr_gov/Documents/Redd_dewatering/Fall_Flow_Redd_Dewatering/External_data/FlowScen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{A0A066C5-4654-4FB4-980C-4BDB5AAFF781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{485B4D85-20D6-444B-BE47-6B344ADFF546}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{A0A066C5-4654-4FB4-980C-4BDB5AAFF781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E86BC56-034B-4BBA-8294-3722716C8166}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="876" activeTab="1" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
+    <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" tabRatio="876" activeTab="5" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Keswick Flow Alternatives" sheetId="3" r:id="rId1"/>
@@ -421,16 +421,16 @@
     <t>Aug 90% WR adj dec</t>
   </si>
   <si>
-    <t>Aug 90% WR dec – Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates. Keswick releases decrease in late September and then increase as demand increases later in October.</t>
+    <t>Aug 90% WR dec = Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates. Keswick releases decrease in late September and then increase as demand increases later in October.</t>
   </si>
   <si>
-    <t>Aug WR 90% flat Dec - Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates. Flows remain at 7,500 cfs in October.</t>
+    <t>Aug 90% WR shape Dec = Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates.  Shifts 500cfs diversion from late Oct to early Oct.</t>
   </si>
   <si>
-    <t>Aug 90% WR shape Dec - Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates.  Shifts 500cfs diversion from late Oct to early Oct.</t>
+    <t>Aug 90% WR adj Dec = Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates. Keswick releases decrease in late September and then increase as demand increases later in October. Flows remain higher in early November to shift diversions later into the season.</t>
   </si>
   <si>
-    <t>Aug 90% adj Dec - Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates. Keswick releases decrease in late September and then increase as demand increases later in October. Flows remain higher in early November to shift diversions later into the season.</t>
+    <t>Aug 90% WR flat Dec = Developed on 9/6/2024. Based on the 90% forecast exceedance. Follows ramping rates. Flows remain at 7,500 cfs in October.</t>
   </si>
 </sst>
 </file>
@@ -1822,6 +1822,20 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1867,20 +1881,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="126">
     <cellStyle name="Comma 10" xfId="86" xr:uid="{18F22F41-CF6B-4170-A614-400F6543E9A0}"/>
@@ -23709,6 +23709,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -24009,36 +24013,36 @@
   <dimension ref="A1:O238"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="J18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="L219" sqref="L219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.36328125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" style="19" customWidth="1"/>
-    <col min="3" max="4" width="7.08984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.90625" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.36328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.08984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.36328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.54296875" style="19" customWidth="1"/>
-    <col min="15" max="15" width="8.54296875" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.54296875" style="19"/>
+    <col min="1" max="1" width="29.33203125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="19" customWidth="1"/>
+    <col min="3" max="4" width="7.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.5546875" style="19" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.5546875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27"/>
     </row>
-    <row r="2" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
@@ -24081,7 +24085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40">
         <f t="shared" ref="A3:A32" si="0">A4-1</f>
         <v>45505</v>
@@ -24118,7 +24122,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40">
         <f t="shared" si="0"/>
         <v>45506</v>
@@ -24161,7 +24165,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="40">
         <f t="shared" si="0"/>
         <v>45507</v>
@@ -24204,7 +24208,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="40">
         <f t="shared" si="0"/>
         <v>45508</v>
@@ -24247,7 +24251,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="40">
         <f t="shared" si="0"/>
         <v>45509</v>
@@ -24290,7 +24294,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="40">
         <f t="shared" si="0"/>
         <v>45510</v>
@@ -24333,7 +24337,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="40">
         <f t="shared" si="0"/>
         <v>45511</v>
@@ -24376,7 +24380,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="40">
         <f t="shared" si="0"/>
         <v>45512</v>
@@ -24419,7 +24423,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <f t="shared" si="0"/>
         <v>45513</v>
@@ -24462,7 +24466,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <f t="shared" si="0"/>
         <v>45514</v>
@@ -24505,7 +24509,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <f t="shared" si="0"/>
         <v>45515</v>
@@ -24548,7 +24552,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <f t="shared" si="0"/>
         <v>45516</v>
@@ -24591,7 +24595,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <f t="shared" si="0"/>
         <v>45517</v>
@@ -24634,7 +24638,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <f t="shared" si="0"/>
         <v>45518</v>
@@ -24677,7 +24681,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <f t="shared" si="0"/>
         <v>45519</v>
@@ -24720,7 +24724,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <f t="shared" si="0"/>
         <v>45520</v>
@@ -24763,7 +24767,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <f t="shared" si="0"/>
         <v>45521</v>
@@ -24806,7 +24810,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <f t="shared" si="0"/>
         <v>45522</v>
@@ -24849,7 +24853,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <f t="shared" si="0"/>
         <v>45523</v>
@@ -24892,7 +24896,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <f t="shared" si="0"/>
         <v>45524</v>
@@ -24935,7 +24939,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
         <f t="shared" si="0"/>
         <v>45525</v>
@@ -24978,7 +24982,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <f t="shared" si="0"/>
         <v>45526</v>
@@ -25021,7 +25025,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <f t="shared" si="0"/>
         <v>45527</v>
@@ -25064,7 +25068,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <f t="shared" si="0"/>
         <v>45528</v>
@@ -25107,7 +25111,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <f t="shared" si="0"/>
         <v>45529</v>
@@ -25150,7 +25154,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <f t="shared" si="0"/>
         <v>45530</v>
@@ -25193,7 +25197,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <f t="shared" si="0"/>
         <v>45531</v>
@@ -25236,7 +25240,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <f t="shared" si="0"/>
         <v>45532</v>
@@ -25279,7 +25283,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <f t="shared" si="0"/>
         <v>45533</v>
@@ -25322,7 +25326,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <f t="shared" si="0"/>
         <v>45534</v>
@@ -25365,7 +25369,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="41">
         <f>A34-1</f>
         <v>45535</v>
@@ -25408,7 +25412,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="54">
         <v>45536</v>
       </c>
@@ -25452,7 +25456,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="42">
         <f>A34+1</f>
         <v>45537</v>
@@ -25503,7 +25507,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="42">
         <f t="shared" ref="A36:A99" si="63">A35+1</f>
         <v>45538</v>
@@ -25554,7 +25558,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="42">
         <f t="shared" si="63"/>
         <v>45539</v>
@@ -25605,7 +25609,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="42">
         <f t="shared" si="63"/>
         <v>45540</v>
@@ -25656,7 +25660,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="42">
         <f t="shared" si="63"/>
         <v>45541</v>
@@ -25707,7 +25711,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="42">
         <f t="shared" si="63"/>
         <v>45542</v>
@@ -25758,7 +25762,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="42">
         <f t="shared" si="63"/>
         <v>45543</v>
@@ -25809,7 +25813,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="42">
         <f t="shared" si="63"/>
         <v>45544</v>
@@ -25860,7 +25864,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="42">
         <f t="shared" si="63"/>
         <v>45545</v>
@@ -25911,7 +25915,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="42">
         <f t="shared" si="63"/>
         <v>45546</v>
@@ -25960,7 +25964,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="42">
         <f t="shared" si="63"/>
         <v>45547</v>
@@ -26009,7 +26013,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="42">
         <f t="shared" si="63"/>
         <v>45548</v>
@@ -26058,7 +26062,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="42">
         <f t="shared" si="63"/>
         <v>45549</v>
@@ -26107,7 +26111,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="42">
         <f t="shared" si="63"/>
         <v>45550</v>
@@ -26156,7 +26160,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="42">
         <f t="shared" si="63"/>
         <v>45551</v>
@@ -26205,7 +26209,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="42">
         <f t="shared" si="63"/>
         <v>45552</v>
@@ -26254,7 +26258,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="42">
         <f t="shared" si="63"/>
         <v>45553</v>
@@ -26303,7 +26307,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="42">
         <f t="shared" si="63"/>
         <v>45554</v>
@@ -26352,7 +26356,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="42">
         <f t="shared" si="63"/>
         <v>45555</v>
@@ -26401,7 +26405,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="42">
         <f t="shared" si="63"/>
         <v>45556</v>
@@ -26450,7 +26454,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="42">
         <f t="shared" si="63"/>
         <v>45557</v>
@@ -26499,7 +26503,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="42">
         <f t="shared" si="63"/>
         <v>45558</v>
@@ -26548,7 +26552,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="42">
         <f t="shared" si="63"/>
         <v>45559</v>
@@ -26597,7 +26601,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="42">
         <f t="shared" si="63"/>
         <v>45560</v>
@@ -26646,7 +26650,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="42">
         <f t="shared" si="63"/>
         <v>45561</v>
@@ -26695,7 +26699,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="42">
         <f t="shared" si="63"/>
         <v>45562</v>
@@ -26744,7 +26748,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="42">
         <f t="shared" si="63"/>
         <v>45563</v>
@@ -26793,7 +26797,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="42">
         <f t="shared" si="63"/>
         <v>45564</v>
@@ -26842,7 +26846,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="42">
         <f t="shared" si="63"/>
         <v>45565</v>
@@ -26891,7 +26895,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="62">
         <f t="shared" si="63"/>
         <v>45566</v>
@@ -26934,7 +26938,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="42">
         <f t="shared" si="63"/>
         <v>45567</v>
@@ -26983,7 +26987,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="42">
         <f t="shared" si="63"/>
         <v>45568</v>
@@ -27032,7 +27036,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="42">
         <f t="shared" si="63"/>
         <v>45569</v>
@@ -27081,7 +27085,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="42">
         <f t="shared" si="63"/>
         <v>45570</v>
@@ -27130,7 +27134,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="42">
         <f t="shared" si="63"/>
         <v>45571</v>
@@ -27179,7 +27183,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="42">
         <f t="shared" si="63"/>
         <v>45572</v>
@@ -27228,7 +27232,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="42">
         <f t="shared" si="63"/>
         <v>45573</v>
@@ -27277,7 +27281,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="42">
         <f t="shared" si="63"/>
         <v>45574</v>
@@ -27326,7 +27330,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="42">
         <f t="shared" si="63"/>
         <v>45575</v>
@@ -27375,7 +27379,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="42">
         <f t="shared" si="63"/>
         <v>45576</v>
@@ -27424,7 +27428,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="42">
         <f t="shared" si="63"/>
         <v>45577</v>
@@ -27473,7 +27477,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="42">
         <f t="shared" si="63"/>
         <v>45578</v>
@@ -27522,7 +27526,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="42">
         <f t="shared" si="63"/>
         <v>45579</v>
@@ -27571,7 +27575,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="42">
         <f t="shared" si="63"/>
         <v>45580</v>
@@ -27620,7 +27624,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="42">
         <f t="shared" si="63"/>
         <v>45581</v>
@@ -27669,7 +27673,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="42">
         <f t="shared" si="63"/>
         <v>45582</v>
@@ -27718,7 +27722,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="42">
         <f t="shared" si="63"/>
         <v>45583</v>
@@ -27767,7 +27771,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="42">
         <f t="shared" si="63"/>
         <v>45584</v>
@@ -27816,7 +27820,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="42">
         <f t="shared" si="63"/>
         <v>45585</v>
@@ -27865,7 +27869,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="42">
         <f t="shared" si="63"/>
         <v>45586</v>
@@ -27914,7 +27918,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="42">
         <f t="shared" si="63"/>
         <v>45587</v>
@@ -27963,7 +27967,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="42">
         <f t="shared" si="63"/>
         <v>45588</v>
@@ -28012,7 +28016,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="42">
         <f t="shared" si="63"/>
         <v>45589</v>
@@ -28061,7 +28065,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="42">
         <f t="shared" si="63"/>
         <v>45590</v>
@@ -28110,7 +28114,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="42">
         <f t="shared" si="63"/>
         <v>45591</v>
@@ -28159,7 +28163,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="42">
         <f t="shared" si="63"/>
         <v>45592</v>
@@ -28208,7 +28212,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="42">
         <f t="shared" si="63"/>
         <v>45593</v>
@@ -28257,7 +28261,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="42">
         <f t="shared" si="63"/>
         <v>45594</v>
@@ -28306,7 +28310,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="42">
         <f t="shared" si="63"/>
         <v>45595</v>
@@ -28355,7 +28359,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="42">
         <f t="shared" si="63"/>
         <v>45596</v>
@@ -28404,7 +28408,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="62">
         <f t="shared" si="63"/>
         <v>45597</v>
@@ -28447,7 +28451,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="43">
         <f t="shared" si="63"/>
         <v>45598</v>
@@ -28495,7 +28499,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="43">
         <f t="shared" si="63"/>
         <v>45599</v>
@@ -28543,7 +28547,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="43">
         <f t="shared" si="63"/>
         <v>45600</v>
@@ -28591,7 +28595,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="43">
         <f t="shared" si="63"/>
         <v>45601</v>
@@ -28639,7 +28643,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="43">
         <f t="shared" ref="A100:A163" si="194">A99+1</f>
         <v>45602</v>
@@ -28687,7 +28691,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="43">
         <f t="shared" si="194"/>
         <v>45603</v>
@@ -28735,7 +28739,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="43">
         <f t="shared" si="194"/>
         <v>45604</v>
@@ -28783,7 +28787,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="43">
         <f t="shared" si="194"/>
         <v>45605</v>
@@ -28833,7 +28837,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="43">
         <f t="shared" si="194"/>
         <v>45606</v>
@@ -28883,7 +28887,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="43">
         <f t="shared" si="194"/>
         <v>45607</v>
@@ -28933,7 +28937,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="43">
         <f t="shared" si="194"/>
         <v>45608</v>
@@ -28983,7 +28987,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="43">
         <f t="shared" si="194"/>
         <v>45609</v>
@@ -29030,7 +29034,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="43">
         <f t="shared" si="194"/>
         <v>45610</v>
@@ -29079,7 +29083,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" s="43">
         <f t="shared" si="194"/>
         <v>45611</v>
@@ -29128,7 +29132,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" s="43">
         <f t="shared" si="194"/>
         <v>45612</v>
@@ -29177,7 +29181,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" s="43">
         <f t="shared" si="194"/>
         <v>45613</v>
@@ -29228,7 +29232,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" s="43">
         <f t="shared" si="194"/>
         <v>45614</v>
@@ -29279,7 +29283,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" s="43">
         <f t="shared" si="194"/>
         <v>45615</v>
@@ -29330,7 +29334,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" s="43">
         <f t="shared" si="194"/>
         <v>45616</v>
@@ -29381,7 +29385,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="43">
         <f t="shared" si="194"/>
         <v>45617</v>
@@ -29432,7 +29436,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="43">
         <f t="shared" si="194"/>
         <v>45618</v>
@@ -29483,7 +29487,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="43">
         <f t="shared" si="194"/>
         <v>45619</v>
@@ -29534,7 +29538,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="43">
         <f t="shared" si="194"/>
         <v>45620</v>
@@ -29585,7 +29589,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" s="43">
         <f t="shared" si="194"/>
         <v>45621</v>
@@ -29636,7 +29640,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" s="43">
         <f t="shared" si="194"/>
         <v>45622</v>
@@ -29687,7 +29691,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" s="43">
         <f t="shared" si="194"/>
         <v>45623</v>
@@ -29738,7 +29742,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" s="43">
         <f t="shared" si="194"/>
         <v>45624</v>
@@ -29789,7 +29793,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" s="43">
         <f t="shared" si="194"/>
         <v>45625</v>
@@ -29840,7 +29844,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" s="44">
         <f t="shared" si="194"/>
         <v>45626</v>
@@ -29891,7 +29895,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" s="54">
         <f t="shared" si="194"/>
         <v>45627</v>
@@ -29934,7 +29938,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" s="42">
         <f t="shared" si="194"/>
         <v>45628</v>
@@ -29987,7 +29991,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" s="42">
         <f t="shared" si="194"/>
         <v>45629</v>
@@ -30040,7 +30044,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" s="42">
         <f t="shared" si="194"/>
         <v>45630</v>
@@ -30093,7 +30097,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" s="42">
         <f t="shared" si="194"/>
         <v>45631</v>
@@ -30146,7 +30150,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" s="42">
         <f t="shared" si="194"/>
         <v>45632</v>
@@ -30199,7 +30203,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" s="42">
         <f t="shared" si="194"/>
         <v>45633</v>
@@ -30252,7 +30256,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" s="42">
         <f t="shared" si="194"/>
         <v>45634</v>
@@ -30305,7 +30309,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" s="42">
         <f t="shared" si="194"/>
         <v>45635</v>
@@ -30358,7 +30362,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" s="42">
         <f t="shared" si="194"/>
         <v>45636</v>
@@ -30411,7 +30415,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" s="42">
         <f t="shared" si="194"/>
         <v>45637</v>
@@ -30464,7 +30468,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" s="42">
         <f t="shared" si="194"/>
         <v>45638</v>
@@ -30517,7 +30521,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="42">
         <f t="shared" si="194"/>
         <v>45639</v>
@@ -30570,7 +30574,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" s="42">
         <f t="shared" si="194"/>
         <v>45640</v>
@@ -30623,7 +30627,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" s="42">
         <f t="shared" si="194"/>
         <v>45641</v>
@@ -30676,7 +30680,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" s="42">
         <f t="shared" si="194"/>
         <v>45642</v>
@@ -30729,7 +30733,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" s="42">
         <f t="shared" si="194"/>
         <v>45643</v>
@@ -30782,7 +30786,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" s="42">
         <f t="shared" si="194"/>
         <v>45644</v>
@@ -30835,7 +30839,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" s="42">
         <f t="shared" si="194"/>
         <v>45645</v>
@@ -30888,7 +30892,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" s="42">
         <f t="shared" si="194"/>
         <v>45646</v>
@@ -30941,7 +30945,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" s="42">
         <f t="shared" si="194"/>
         <v>45647</v>
@@ -30994,7 +30998,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" s="42">
         <f t="shared" si="194"/>
         <v>45648</v>
@@ -31047,7 +31051,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" s="42">
         <f t="shared" si="194"/>
         <v>45649</v>
@@ -31100,7 +31104,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" s="42">
         <f t="shared" si="194"/>
         <v>45650</v>
@@ -31153,7 +31157,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" s="42">
         <f t="shared" si="194"/>
         <v>45651</v>
@@ -31206,7 +31210,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" s="42">
         <f t="shared" si="194"/>
         <v>45652</v>
@@ -31259,7 +31263,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" s="42">
         <f t="shared" si="194"/>
         <v>45653</v>
@@ -31312,7 +31316,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" s="42">
         <f t="shared" si="194"/>
         <v>45654</v>
@@ -31365,7 +31369,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" s="42">
         <f t="shared" si="194"/>
         <v>45655</v>
@@ -31418,7 +31422,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" s="42">
         <f t="shared" si="194"/>
         <v>45656</v>
@@ -31471,7 +31475,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" s="42">
         <f t="shared" si="194"/>
         <v>45657</v>
@@ -31524,7 +31528,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" s="62">
         <f t="shared" si="194"/>
         <v>45658</v>
@@ -31567,7 +31571,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" s="43">
         <f t="shared" si="194"/>
         <v>45659</v>
@@ -31620,7 +31624,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" s="43">
         <f t="shared" si="194"/>
         <v>45660</v>
@@ -31673,7 +31677,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" s="43">
         <f t="shared" si="194"/>
         <v>45661</v>
@@ -31726,7 +31730,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" s="43">
         <f t="shared" si="194"/>
         <v>45662</v>
@@ -31779,7 +31783,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" s="43">
         <f t="shared" si="194"/>
         <v>45663</v>
@@ -31832,7 +31836,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" s="43">
         <f t="shared" si="194"/>
         <v>45664</v>
@@ -31885,7 +31889,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" s="43">
         <f t="shared" si="194"/>
         <v>45665</v>
@@ -31938,7 +31942,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" s="43">
         <f t="shared" ref="A164:A214" si="499">A163+1</f>
         <v>45666</v>
@@ -31991,7 +31995,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" s="43">
         <f t="shared" si="499"/>
         <v>45667</v>
@@ -32044,7 +32048,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" s="43">
         <f t="shared" si="499"/>
         <v>45668</v>
@@ -32097,7 +32101,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" s="43">
         <f t="shared" si="499"/>
         <v>45669</v>
@@ -32150,7 +32154,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" s="43">
         <f t="shared" si="499"/>
         <v>45670</v>
@@ -32203,7 +32207,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" s="43">
         <f t="shared" si="499"/>
         <v>45671</v>
@@ -32256,7 +32260,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" s="43">
         <f t="shared" si="499"/>
         <v>45672</v>
@@ -32309,7 +32313,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" s="43">
         <f t="shared" si="499"/>
         <v>45673</v>
@@ -32362,7 +32366,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" s="43">
         <f t="shared" si="499"/>
         <v>45674</v>
@@ -32415,7 +32419,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" s="43">
         <f t="shared" si="499"/>
         <v>45675</v>
@@ -32468,7 +32472,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" s="43">
         <f t="shared" si="499"/>
         <v>45676</v>
@@ -32521,7 +32525,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" s="43">
         <f t="shared" si="499"/>
         <v>45677</v>
@@ -32574,7 +32578,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" s="43">
         <f t="shared" si="499"/>
         <v>45678</v>
@@ -32627,7 +32631,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" s="43">
         <f t="shared" si="499"/>
         <v>45679</v>
@@ -32680,7 +32684,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A178" s="43">
         <f t="shared" si="499"/>
         <v>45680</v>
@@ -32733,7 +32737,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" s="43">
         <f t="shared" si="499"/>
         <v>45681</v>
@@ -32786,7 +32790,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" s="43">
         <f t="shared" si="499"/>
         <v>45682</v>
@@ -32839,7 +32843,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" s="43">
         <f t="shared" si="499"/>
         <v>45683</v>
@@ -32892,7 +32896,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" s="43">
         <f t="shared" si="499"/>
         <v>45684</v>
@@ -32945,7 +32949,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" s="43">
         <f t="shared" si="499"/>
         <v>45685</v>
@@ -32998,7 +33002,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" s="43">
         <f t="shared" si="499"/>
         <v>45686</v>
@@ -33051,7 +33055,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" s="43">
         <f t="shared" si="499"/>
         <v>45687</v>
@@ -33104,7 +33108,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" s="44">
         <f t="shared" si="499"/>
         <v>45688</v>
@@ -33157,7 +33161,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" s="54">
         <f t="shared" si="499"/>
         <v>45689</v>
@@ -33200,7 +33204,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A188" s="42">
         <f t="shared" si="499"/>
         <v>45690</v>
@@ -33253,7 +33257,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" s="42">
         <f t="shared" si="499"/>
         <v>45691</v>
@@ -33306,7 +33310,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A190" s="42">
         <f t="shared" si="499"/>
         <v>45692</v>
@@ -33359,7 +33363,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" s="42">
         <f t="shared" si="499"/>
         <v>45693</v>
@@ -33412,7 +33416,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" s="42">
         <f t="shared" si="499"/>
         <v>45694</v>
@@ -33465,7 +33469,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" s="42">
         <f t="shared" si="499"/>
         <v>45695</v>
@@ -33518,7 +33522,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A194" s="42">
         <f t="shared" si="499"/>
         <v>45696</v>
@@ -33571,7 +33575,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" s="42">
         <f t="shared" si="499"/>
         <v>45697</v>
@@ -33624,7 +33628,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" s="42">
         <f t="shared" si="499"/>
         <v>45698</v>
@@ -33677,7 +33681,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" s="42">
         <f t="shared" si="499"/>
         <v>45699</v>
@@ -33730,7 +33734,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" s="42">
         <f t="shared" si="499"/>
         <v>45700</v>
@@ -33783,7 +33787,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" s="42">
         <f t="shared" si="499"/>
         <v>45701</v>
@@ -33836,7 +33840,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" s="42">
         <f t="shared" si="499"/>
         <v>45702</v>
@@ -33889,7 +33893,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" s="42">
         <f t="shared" si="499"/>
         <v>45703</v>
@@ -33942,7 +33946,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A202" s="42">
         <f t="shared" si="499"/>
         <v>45704</v>
@@ -33995,7 +33999,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" s="42">
         <f t="shared" si="499"/>
         <v>45705</v>
@@ -34048,7 +34052,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A204" s="42">
         <f t="shared" si="499"/>
         <v>45706</v>
@@ -34101,7 +34105,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A205" s="42">
         <f t="shared" si="499"/>
         <v>45707</v>
@@ -34154,7 +34158,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A206" s="42">
         <f t="shared" si="499"/>
         <v>45708</v>
@@ -34207,7 +34211,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A207" s="42">
         <f t="shared" si="499"/>
         <v>45709</v>
@@ -34260,7 +34264,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A208" s="42">
         <f t="shared" si="499"/>
         <v>45710</v>
@@ -34313,7 +34317,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A209" s="42">
         <f t="shared" si="499"/>
         <v>45711</v>
@@ -34366,7 +34370,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A210" s="42">
         <f t="shared" si="499"/>
         <v>45712</v>
@@ -34419,7 +34423,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A211" s="42">
         <f t="shared" si="499"/>
         <v>45713</v>
@@ -34472,7 +34476,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A212" s="42">
         <f t="shared" si="499"/>
         <v>45714</v>
@@ -34525,7 +34529,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A213" s="42">
         <f t="shared" si="499"/>
         <v>45715</v>
@@ -34578,7 +34582,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A214" s="42">
         <f t="shared" si="499"/>
         <v>45716</v>
@@ -34631,7 +34635,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A215" s="42"/>
       <c r="B215" s="31"/>
       <c r="C215" s="22"/>
@@ -34648,7 +34652,7 @@
       <c r="N215" s="21"/>
       <c r="O215" s="29"/>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A216" s="34"/>
       <c r="B216" s="34"/>
       <c r="C216" s="23"/>
@@ -34663,7 +34667,7 @@
       <c r="M216" s="23"/>
       <c r="N216" s="23"/>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A217" s="45" t="s">
         <v>10</v>
       </c>
@@ -34717,7 +34721,7 @@
       </c>
       <c r="N217" s="24"/>
     </row>
-    <row r="218" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="37" t="s">
         <v>11</v>
       </c>
@@ -34768,7 +34772,7 @@
       </c>
       <c r="N218" s="24"/>
     </row>
-    <row r="219" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="17" t="s">
         <v>12</v>
       </c>
@@ -34819,7 +34823,7 @@
       </c>
       <c r="N219" s="24"/>
     </row>
-    <row r="220" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="17" t="s">
         <v>13</v>
       </c>
@@ -34870,7 +34874,7 @@
       </c>
       <c r="N220" s="24"/>
     </row>
-    <row r="221" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="17" t="s">
         <v>14</v>
       </c>
@@ -34921,7 +34925,7 @@
       </c>
       <c r="N221" s="24"/>
     </row>
-    <row r="222" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="17" t="s">
         <v>15</v>
       </c>
@@ -34972,7 +34976,7 @@
       </c>
       <c r="N222" s="24"/>
     </row>
-    <row r="223" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="17" t="s">
         <v>16</v>
       </c>
@@ -35023,7 +35027,7 @@
       </c>
       <c r="N223" s="24"/>
     </row>
-    <row r="224" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="17" t="s">
         <v>17</v>
       </c>
@@ -35041,7 +35045,7 @@
       <c r="M224" s="24"/>
       <c r="N224" s="24"/>
     </row>
-    <row r="225" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="17" t="s">
         <v>18</v>
       </c>
@@ -35092,7 +35096,7 @@
       </c>
       <c r="N225" s="24"/>
     </row>
-    <row r="226" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="17" t="s">
         <v>19</v>
       </c>
@@ -35143,7 +35147,7 @@
       </c>
       <c r="N226" s="24"/>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A227" s="17" t="s">
         <v>20</v>
       </c>
@@ -35194,7 +35198,7 @@
       </c>
       <c r="N227" s="24"/>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A228" s="17" t="s">
         <v>21</v>
       </c>
@@ -35245,7 +35249,7 @@
       </c>
       <c r="N228" s="24"/>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A229" s="17" t="s">
         <v>22</v>
       </c>
@@ -35295,7 +35299,7 @@
       </c>
       <c r="N229" s="24"/>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A230" s="17" t="s">
         <v>23</v>
       </c>
@@ -35345,7 +35349,7 @@
       </c>
       <c r="N230" s="24"/>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A231" s="17" t="s">
         <v>24</v>
       </c>
@@ -35395,7 +35399,7 @@
       </c>
       <c r="N231" s="23"/>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A233" s="17" t="s">
         <v>91</v>
       </c>
@@ -35406,7 +35410,7 @@
         <v>2717</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A234" s="17" t="s">
         <v>89</v>
       </c>
@@ -35417,7 +35421,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A235" s="17" t="s">
         <v>90</v>
       </c>
@@ -35428,7 +35432,7 @@
         <v>2570</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A236" s="17" t="s">
         <v>92</v>
       </c>
@@ -35439,7 +35443,7 @@
         <v>2643</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A237" s="17" t="s">
         <v>93</v>
       </c>
@@ -35450,7 +35454,7 @@
         <v>2713</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A238" s="17" t="s">
         <v>94</v>
       </c>
@@ -35474,16 +35478,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D67B6F-CD3E-42CC-BABC-E7E74F1F1B54}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="152" t="s">
         <v>25</v>
       </c>
@@ -35491,7 +35495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="str">
         <f>'Keswick Flow Alternatives'!C2</f>
         <v>Jul 50%</v>
@@ -35500,7 +35504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="str">
         <f>'Keswick Flow Alternatives'!D2</f>
         <v>Jul 90%</v>
@@ -35509,7 +35513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="str">
         <f>'Keswick Flow Alternatives'!E2</f>
         <v>Aug 50%</v>
@@ -35518,7 +35522,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="str">
         <f>'Keswick Flow Alternatives'!F2</f>
         <v>Aug 90%</v>
@@ -35527,7 +35531,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="str">
         <f>'Keswick Flow Alternatives'!G2</f>
         <v>Aug 50% WR1</v>
@@ -35536,7 +35540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="str">
         <f>'Keswick Flow Alternatives'!H2</f>
         <v>Aug 90% WR1</v>
@@ -35545,7 +35549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="str">
         <f>'Keswick Flow Alternatives'!I2</f>
         <v>Aug 90% WR dec</v>
@@ -35554,7 +35558,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="str">
         <f>'Keswick Flow Alternatives'!J2</f>
         <v>Aug 90% WR flat dec</v>
@@ -35563,7 +35567,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="str">
         <f>'Keswick Flow Alternatives'!K2</f>
         <v>Aug 90% WR shape dec</v>
@@ -35572,7 +35576,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="str">
         <f>'Keswick Flow Alternatives'!L2</f>
         <v>Aug 90% WR adj dec</v>
@@ -35581,7 +35585,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <f>'Keswick Flow Alternatives'!M2</f>
         <v>0</v>
@@ -35590,7 +35594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <f>'Keswick Flow Alternatives'!N2</f>
         <v>0</v>
@@ -35599,22 +35603,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="20"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="20"/>
     </row>
   </sheetData>
@@ -35630,60 +35634,60 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49"/>
     </row>
-    <row r="3" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="51" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="51"/>
     </row>
-    <row r="5" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="51"/>
     </row>
-    <row r="7" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="48"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="48"/>
     </row>
-    <row r="11" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="50"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="52" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -35698,133 +35702,133 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA370860-48CD-4B92-B790-82066B2C7AEE}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="13.44140625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="61" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="61" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="61" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="61" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" s="25" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" s="25" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="61" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="61" t="s">
         <v>99</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="157" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="158" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="158" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="158" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="39"/>
     </row>
   </sheetData>
@@ -35840,56 +35844,56 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
-    <col min="10" max="10" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A1" s="168" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A1" s="178" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="168" t="s">
+      <c r="B1" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="168" t="s">
+      <c r="C1" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="168" t="s">
+      <c r="D1" s="178" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="168" t="s">
+      <c r="E1" s="178" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="168" t="s">
+      <c r="F1" s="178" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="168" t="s">
+      <c r="G1" s="178" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="168" t="s">
+      <c r="H1" s="178" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="168" t="s">
+      <c r="I1" s="178" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="168" t="s">
+      <c r="J1" s="178" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="171" t="s">
+      <c r="K1" s="181" t="s">
         <v>59</v>
       </c>
       <c r="L1" s="64"/>
       <c r="M1" s="64"/>
-      <c r="N1" s="159" t="s">
+      <c r="N1" s="169" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="160"/>
-      <c r="P1" s="163" t="s">
+      <c r="O1" s="170"/>
+      <c r="P1" s="173" t="s">
         <v>61</v>
       </c>
       <c r="Q1" s="65">
@@ -35931,23 +35935,23 @@
       <c r="AI1" s="64"/>
       <c r="AJ1" s="64"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A2" s="169"/>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="172"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A2" s="179"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="179"/>
+      <c r="K2" s="182"/>
       <c r="L2" s="64"/>
       <c r="M2" s="64"/>
-      <c r="N2" s="161"/>
-      <c r="O2" s="162"/>
-      <c r="P2" s="164"/>
+      <c r="N2" s="171"/>
+      <c r="O2" s="172"/>
+      <c r="P2" s="174"/>
       <c r="Q2" s="72">
         <v>45445</v>
       </c>
@@ -35987,36 +35991,36 @@
       <c r="AI2" s="64"/>
       <c r="AJ2" s="64"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A3" s="169"/>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="172"/>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A3" s="179"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="182"/>
       <c r="L3" s="64"/>
       <c r="M3" s="64"/>
-      <c r="N3" s="165" t="s">
-        <v>62</v>
-      </c>
-      <c r="O3" s="166"/>
-      <c r="P3" s="167"/>
-      <c r="Q3" s="174" t="s">
+      <c r="N3" s="175" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="176"/>
+      <c r="P3" s="177"/>
+      <c r="Q3" s="163" t="s">
         <v>63</v>
       </c>
-      <c r="R3" s="174"/>
-      <c r="S3" s="174"/>
-      <c r="T3" s="174"/>
-      <c r="U3" s="174"/>
-      <c r="V3" s="174"/>
-      <c r="W3" s="174"/>
-      <c r="X3" s="174"/>
-      <c r="Y3" s="175"/>
+      <c r="R3" s="163"/>
+      <c r="S3" s="163"/>
+      <c r="T3" s="163"/>
+      <c r="U3" s="163"/>
+      <c r="V3" s="163"/>
+      <c r="W3" s="163"/>
+      <c r="X3" s="163"/>
+      <c r="Y3" s="164"/>
       <c r="Z3" s="77"/>
       <c r="AA3" s="77"/>
       <c r="AB3" s="77"/>
@@ -36029,18 +36033,18 @@
       <c r="AI3" s="77"/>
       <c r="AJ3" s="77"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A4" s="170"/>
-      <c r="B4" s="170"/>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="170"/>
-      <c r="J4" s="170"/>
-      <c r="K4" s="173"/>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A4" s="180"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="183"/>
       <c r="L4" s="64"/>
       <c r="M4" s="78" t="s">
         <v>62</v>
@@ -36048,10 +36052,10 @@
       <c r="N4" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="O4" s="176" t="s">
+      <c r="O4" s="165" t="s">
         <v>65</v>
       </c>
-      <c r="P4" s="177"/>
+      <c r="P4" s="166"/>
       <c r="Q4" s="80">
         <v>8700</v>
       </c>
@@ -36091,7 +36095,7 @@
       <c r="AI4" s="64"/>
       <c r="AJ4" s="64"/>
     </row>
-    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="85">
         <v>1</v>
       </c>
@@ -36134,10 +36138,10 @@
       <c r="N5" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="178">
+      <c r="O5" s="167">
         <v>26</v>
       </c>
-      <c r="P5" s="179"/>
+      <c r="P5" s="168"/>
       <c r="Q5" s="67">
         <v>26</v>
       </c>
@@ -36177,7 +36181,7 @@
       <c r="AI5" s="64"/>
       <c r="AJ5" s="64"/>
     </row>
-    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="85">
         <v>2</v>
       </c>
@@ -36220,10 +36224,10 @@
       <c r="N6" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="180">
+      <c r="O6" s="159">
         <v>27</v>
       </c>
-      <c r="P6" s="181"/>
+      <c r="P6" s="160"/>
       <c r="Q6" s="97" t="s">
         <v>62</v>
       </c>
@@ -36263,7 +36267,7 @@
       <c r="AI6" s="64"/>
       <c r="AJ6" s="64"/>
     </row>
-    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="85">
         <v>3</v>
       </c>
@@ -36306,10 +36310,10 @@
       <c r="N7" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="O7" s="180">
+      <c r="O7" s="159">
         <v>23</v>
       </c>
-      <c r="P7" s="181"/>
+      <c r="P7" s="160"/>
       <c r="Q7" s="97" t="s">
         <v>62</v>
       </c>
@@ -36351,7 +36355,7 @@
       <c r="AI7" s="64"/>
       <c r="AJ7" s="64"/>
     </row>
-    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="85">
         <v>4</v>
       </c>
@@ -36394,10 +36398,10 @@
       <c r="N8" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="O8" s="180">
+      <c r="O8" s="159">
         <v>13</v>
       </c>
-      <c r="P8" s="181"/>
+      <c r="P8" s="160"/>
       <c r="Q8" s="97" t="s">
         <v>62</v>
       </c>
@@ -36439,7 +36443,7 @@
       <c r="AI8" s="64"/>
       <c r="AJ8" s="64"/>
     </row>
-    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="85">
         <v>5</v>
       </c>
@@ -36482,10 +36486,10 @@
       <c r="N9" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="O9" s="180">
+      <c r="O9" s="159">
         <v>22</v>
       </c>
-      <c r="P9" s="181"/>
+      <c r="P9" s="160"/>
       <c r="Q9" s="97" t="s">
         <v>62</v>
       </c>
@@ -36525,7 +36529,7 @@
       <c r="AI9" s="64"/>
       <c r="AJ9" s="64"/>
     </row>
-    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="85">
         <v>6</v>
       </c>
@@ -36568,10 +36572,10 @@
       <c r="N10" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="180">
+      <c r="O10" s="159">
         <v>10</v>
       </c>
-      <c r="P10" s="181"/>
+      <c r="P10" s="160"/>
       <c r="Q10" s="97" t="s">
         <v>62</v>
       </c>
@@ -36611,7 +36615,7 @@
       <c r="AI10" s="64"/>
       <c r="AJ10" s="64"/>
     </row>
-    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="85">
         <v>7</v>
       </c>
@@ -36654,10 +36658,10 @@
       <c r="N11" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="O11" s="180">
+      <c r="O11" s="159">
         <v>23</v>
       </c>
-      <c r="P11" s="181"/>
+      <c r="P11" s="160"/>
       <c r="Q11" s="97" t="s">
         <v>62</v>
       </c>
@@ -36697,7 +36701,7 @@
       <c r="AI11" s="64"/>
       <c r="AJ11" s="64"/>
     </row>
-    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="85">
         <v>8</v>
       </c>
@@ -36740,10 +36744,10 @@
       <c r="N12" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="O12" s="180">
+      <c r="O12" s="159">
         <v>34</v>
       </c>
-      <c r="P12" s="181"/>
+      <c r="P12" s="160"/>
       <c r="Q12" s="97" t="s">
         <v>62</v>
       </c>
@@ -36783,7 +36787,7 @@
       <c r="AI12" s="64"/>
       <c r="AJ12" s="64"/>
     </row>
-    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="85">
         <v>9</v>
       </c>
@@ -36826,10 +36830,10 @@
       <c r="N13" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="180">
+      <c r="O13" s="159">
         <v>26</v>
       </c>
-      <c r="P13" s="181"/>
+      <c r="P13" s="160"/>
       <c r="Q13" s="97" t="s">
         <v>62</v>
       </c>
@@ -36869,7 +36873,7 @@
       <c r="AI13" s="64"/>
       <c r="AJ13" s="64"/>
     </row>
-    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="85">
         <v>10</v>
       </c>
@@ -36912,10 +36916,10 @@
       <c r="N14" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="O14" s="180">
+      <c r="O14" s="159">
         <v>25</v>
       </c>
-      <c r="P14" s="181"/>
+      <c r="P14" s="160"/>
       <c r="Q14" s="97" t="s">
         <v>62</v>
       </c>
@@ -36957,7 +36961,7 @@
       <c r="AI14" s="64"/>
       <c r="AJ14" s="64"/>
     </row>
-    <row r="15" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="85">
         <v>11</v>
       </c>
@@ -37000,10 +37004,10 @@
       <c r="N15" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="O15" s="180">
+      <c r="O15" s="159">
         <v>27</v>
       </c>
-      <c r="P15" s="181"/>
+      <c r="P15" s="160"/>
       <c r="Q15" s="97" t="s">
         <v>62</v>
       </c>
@@ -37045,7 +37049,7 @@
       <c r="AI15" s="64"/>
       <c r="AJ15" s="64"/>
     </row>
-    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="85">
         <v>12</v>
       </c>
@@ -37088,10 +37092,10 @@
       <c r="N16" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="O16" s="180">
+      <c r="O16" s="159">
         <v>18</v>
       </c>
-      <c r="P16" s="181"/>
+      <c r="P16" s="160"/>
       <c r="Q16" s="97" t="s">
         <v>62</v>
       </c>
@@ -37131,7 +37135,7 @@
       <c r="AI16" s="64"/>
       <c r="AJ16" s="64"/>
     </row>
-    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="85">
         <v>13</v>
       </c>
@@ -37174,10 +37178,10 @@
       <c r="N17" s="107" t="s">
         <v>84</v>
       </c>
-      <c r="O17" s="180">
+      <c r="O17" s="159">
         <v>34</v>
       </c>
-      <c r="P17" s="181"/>
+      <c r="P17" s="160"/>
       <c r="Q17" s="97" t="s">
         <v>62</v>
       </c>
@@ -37217,7 +37221,7 @@
       <c r="AI17" s="64"/>
       <c r="AJ17" s="64"/>
     </row>
-    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="85">
         <v>14</v>
       </c>
@@ -37260,10 +37264,10 @@
       <c r="N18" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="O18" s="180">
+      <c r="O18" s="159">
         <v>14</v>
       </c>
-      <c r="P18" s="181"/>
+      <c r="P18" s="160"/>
       <c r="Q18" s="97" t="s">
         <v>62</v>
       </c>
@@ -37305,7 +37309,7 @@
       <c r="AI18" s="64"/>
       <c r="AJ18" s="64"/>
     </row>
-    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="85">
         <v>15</v>
       </c>
@@ -37348,10 +37352,10 @@
       <c r="N19" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="O19" s="180">
+      <c r="O19" s="159">
         <v>16</v>
       </c>
-      <c r="P19" s="181"/>
+      <c r="P19" s="160"/>
       <c r="Q19" s="97" t="s">
         <v>62</v>
       </c>
@@ -37393,7 +37397,7 @@
       <c r="AI19" s="64"/>
       <c r="AJ19" s="64"/>
     </row>
-    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="85">
         <v>16</v>
       </c>
@@ -37436,10 +37440,10 @@
       <c r="N20" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="O20" s="180">
+      <c r="O20" s="159">
         <v>24</v>
       </c>
-      <c r="P20" s="181"/>
+      <c r="P20" s="160"/>
       <c r="Q20" s="97" t="s">
         <v>62</v>
       </c>
@@ -37479,7 +37483,7 @@
       <c r="AI20" s="64"/>
       <c r="AJ20" s="64"/>
     </row>
-    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="85" t="s">
         <v>62</v>
       </c>
@@ -37522,10 +37526,10 @@
       <c r="N21" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="O21" s="180" t="s">
-        <v>62</v>
-      </c>
-      <c r="P21" s="181"/>
+      <c r="O21" s="159" t="s">
+        <v>62</v>
+      </c>
+      <c r="P21" s="160"/>
       <c r="Q21" s="97" t="s">
         <v>62</v>
       </c>
@@ -37565,7 +37569,7 @@
       <c r="AI21" s="64"/>
       <c r="AJ21" s="64"/>
     </row>
-    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="85" t="s">
         <v>62</v>
       </c>
@@ -37608,10 +37612,10 @@
       <c r="N22" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="O22" s="180" t="s">
-        <v>62</v>
-      </c>
-      <c r="P22" s="181"/>
+      <c r="O22" s="159" t="s">
+        <v>62</v>
+      </c>
+      <c r="P22" s="160"/>
       <c r="Q22" s="97" t="s">
         <v>62</v>
       </c>
@@ -37651,7 +37655,7 @@
       <c r="AI22" s="64"/>
       <c r="AJ22" s="64"/>
     </row>
-    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="85" t="s">
         <v>62</v>
       </c>
@@ -37694,10 +37698,10 @@
       <c r="N23" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="O23" s="180" t="s">
-        <v>62</v>
-      </c>
-      <c r="P23" s="181"/>
+      <c r="O23" s="159" t="s">
+        <v>62</v>
+      </c>
+      <c r="P23" s="160"/>
       <c r="Q23" s="97" t="s">
         <v>62</v>
       </c>
@@ -37737,7 +37741,7 @@
       <c r="AI23" s="64"/>
       <c r="AJ23" s="64"/>
     </row>
-    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="85" t="s">
         <v>62</v>
       </c>
@@ -37780,10 +37784,10 @@
       <c r="N24" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="O24" s="180" t="s">
-        <v>62</v>
-      </c>
-      <c r="P24" s="181"/>
+      <c r="O24" s="159" t="s">
+        <v>62</v>
+      </c>
+      <c r="P24" s="160"/>
       <c r="Q24" s="97" t="s">
         <v>62</v>
       </c>
@@ -37823,7 +37827,7 @@
       <c r="AI24" s="64"/>
       <c r="AJ24" s="64"/>
     </row>
-    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="85" t="s">
         <v>62</v>
       </c>
@@ -37866,10 +37870,10 @@
       <c r="N25" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="O25" s="180" t="s">
-        <v>62</v>
-      </c>
-      <c r="P25" s="181"/>
+      <c r="O25" s="159" t="s">
+        <v>62</v>
+      </c>
+      <c r="P25" s="160"/>
       <c r="Q25" s="97" t="s">
         <v>62</v>
       </c>
@@ -37909,7 +37913,7 @@
       <c r="AI25" s="64"/>
       <c r="AJ25" s="64"/>
     </row>
-    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="85" t="s">
         <v>62</v>
       </c>
@@ -37952,10 +37956,10 @@
       <c r="N26" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="O26" s="182" t="s">
-        <v>62</v>
-      </c>
-      <c r="P26" s="183"/>
+      <c r="O26" s="161" t="s">
+        <v>62</v>
+      </c>
+      <c r="P26" s="162"/>
       <c r="Q26" s="124" t="s">
         <v>62</v>
       </c>
@@ -37995,7 +37999,7 @@
       <c r="AI26" s="64"/>
       <c r="AJ26" s="64"/>
     </row>
-    <row r="27" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="128" t="s">
         <v>62</v>
       </c>
@@ -38083,7 +38087,7 @@
       <c r="AI27" s="64"/>
       <c r="AJ27" s="64"/>
     </row>
-    <row r="28" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="128" t="s">
         <v>62</v>
       </c>
@@ -38171,7 +38175,7 @@
       <c r="AI28" s="64"/>
       <c r="AJ28" s="64"/>
     </row>
-    <row r="29" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="128" t="s">
         <v>62</v>
       </c>
@@ -38259,7 +38263,7 @@
       <c r="AI29" s="64"/>
       <c r="AJ29" s="64"/>
     </row>
-    <row r="30" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="128" t="s">
         <v>62</v>
       </c>
@@ -38347,7 +38351,7 @@
       <c r="AI30" s="64"/>
       <c r="AJ30" s="64"/>
     </row>
-    <row r="31" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="128" t="s">
         <v>62</v>
       </c>
@@ -38435,7 +38439,7 @@
       <c r="AI31" s="64"/>
       <c r="AJ31" s="64"/>
     </row>
-    <row r="32" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="140" t="s">
         <v>62</v>
       </c>
@@ -38523,7 +38527,7 @@
       <c r="AI32" s="64"/>
       <c r="AJ32" s="64"/>
     </row>
-    <row r="33" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="140" t="s">
         <v>62</v>
       </c>
@@ -38611,7 +38615,7 @@
       <c r="AI33" s="64"/>
       <c r="AJ33" s="64"/>
     </row>
-    <row r="34" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="140" t="s">
         <v>62</v>
       </c>
@@ -38699,7 +38703,7 @@
       <c r="AI34" s="64"/>
       <c r="AJ34" s="64"/>
     </row>
-    <row r="35" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="140" t="s">
         <v>62</v>
       </c>
@@ -38787,7 +38791,7 @@
       <c r="AI35" s="64"/>
       <c r="AJ35" s="64"/>
     </row>
-    <row r="36" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="140" t="s">
         <v>62</v>
       </c>
@@ -38875,7 +38879,7 @@
       <c r="AI36" s="64"/>
       <c r="AJ36" s="64"/>
     </row>
-    <row r="37" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="145" t="s">
         <v>62</v>
       </c>
@@ -38963,7 +38967,7 @@
       <c r="AI37" s="64"/>
       <c r="AJ37" s="64"/>
     </row>
-    <row r="38" spans="1:36" ht="18" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:36" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="145" t="s">
         <v>62</v>
       </c>
@@ -39051,7 +39055,7 @@
       <c r="AI38" s="64"/>
       <c r="AJ38" s="64"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A39" s="145" t="s">
         <v>62</v>
       </c>
@@ -39139,7 +39143,7 @@
       <c r="AI39" s="64"/>
       <c r="AJ39" s="64"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A40" s="145" t="s">
         <v>62</v>
       </c>
@@ -39227,7 +39231,7 @@
       <c r="AI40" s="64"/>
       <c r="AJ40" s="64"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A41" s="145" t="s">
         <v>62</v>
       </c>
@@ -39315,7 +39319,7 @@
       <c r="AI41" s="64"/>
       <c r="AJ41" s="64"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A42" s="145" t="s">
         <v>62</v>
       </c>
@@ -39403,7 +39407,7 @@
       <c r="AI42" s="64"/>
       <c r="AJ42" s="64"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A43" s="145" t="s">
         <v>62</v>
       </c>
@@ -39491,7 +39495,7 @@
       <c r="AI43" s="64"/>
       <c r="AJ43" s="64"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A44" s="145" t="s">
         <v>62</v>
       </c>
@@ -39579,7 +39583,7 @@
       <c r="AI44" s="64"/>
       <c r="AJ44" s="64"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A45" s="145" t="s">
         <v>62</v>
       </c>
@@ -39667,7 +39671,7 @@
       <c r="AI45" s="64"/>
       <c r="AJ45" s="64"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A46" s="145" t="s">
         <v>62</v>
       </c>
@@ -39755,7 +39759,7 @@
       <c r="AI46" s="64"/>
       <c r="AJ46" s="64"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A47" s="145" t="s">
         <v>62</v>
       </c>
@@ -39843,7 +39847,7 @@
       <c r="AI47" s="64"/>
       <c r="AJ47" s="64"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A48" s="145" t="s">
         <v>62</v>
       </c>
@@ -39931,7 +39935,7 @@
       <c r="AI48" s="64"/>
       <c r="AJ48" s="64"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A49" s="145" t="s">
         <v>62</v>
       </c>
@@ -40019,7 +40023,7 @@
       <c r="AI49" s="64"/>
       <c r="AJ49" s="64"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A50" s="145" t="s">
         <v>62</v>
       </c>
@@ -40107,7 +40111,7 @@
       <c r="AI50" s="64"/>
       <c r="AJ50" s="64"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A51" s="145" t="s">
         <v>62</v>
       </c>
@@ -40195,7 +40199,7 @@
       <c r="AI51" s="64"/>
       <c r="AJ51" s="64"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A52" s="145" t="s">
         <v>62</v>
       </c>
@@ -40283,7 +40287,7 @@
       <c r="AI52" s="64"/>
       <c r="AJ52" s="64"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A53" s="145" t="s">
         <v>62</v>
       </c>
@@ -40371,7 +40375,7 @@
       <c r="AI53" s="64"/>
       <c r="AJ53" s="64"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A54" s="145" t="s">
         <v>62</v>
       </c>
@@ -40459,7 +40463,7 @@
       <c r="AI54" s="64"/>
       <c r="AJ54" s="64"/>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A55" s="145" t="s">
         <v>62</v>
       </c>
@@ -40547,7 +40551,7 @@
       <c r="AI55" s="64"/>
       <c r="AJ55" s="64"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A56" s="145" t="s">
         <v>62</v>
       </c>
@@ -40635,7 +40639,7 @@
       <c r="AI56" s="64"/>
       <c r="AJ56" s="64"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A57" s="145" t="s">
         <v>62</v>
       </c>
@@ -40723,7 +40727,7 @@
       <c r="AI57" s="64"/>
       <c r="AJ57" s="64"/>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A58" s="145" t="s">
         <v>62</v>
       </c>
@@ -40811,7 +40815,7 @@
       <c r="AI58" s="64"/>
       <c r="AJ58" s="64"/>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A59" s="145" t="s">
         <v>62</v>
       </c>
@@ -40899,7 +40903,7 @@
       <c r="AI59" s="64"/>
       <c r="AJ59" s="64"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A60" s="145" t="s">
         <v>62</v>
       </c>
@@ -40987,7 +40991,7 @@
       <c r="AI60" s="64"/>
       <c r="AJ60" s="64"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A61" s="145" t="s">
         <v>62</v>
       </c>
@@ -41075,7 +41079,7 @@
       <c r="AI61" s="64"/>
       <c r="AJ61" s="64"/>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A62" s="145" t="s">
         <v>62</v>
       </c>
@@ -41163,7 +41167,7 @@
       <c r="AI62" s="64"/>
       <c r="AJ62" s="64"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A63" s="145" t="s">
         <v>62</v>
       </c>
@@ -41251,7 +41255,7 @@
       <c r="AI63" s="64"/>
       <c r="AJ63" s="64"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A64" s="145" t="s">
         <v>62</v>
       </c>
@@ -41339,7 +41343,7 @@
       <c r="AI64" s="64"/>
       <c r="AJ64" s="64"/>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A65" s="145" t="s">
         <v>62</v>
       </c>
@@ -41427,7 +41431,7 @@
       <c r="AI65" s="64"/>
       <c r="AJ65" s="64"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A66" s="145" t="s">
         <v>62</v>
       </c>
@@ -41515,7 +41519,7 @@
       <c r="AI66" s="64"/>
       <c r="AJ66" s="64"/>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A67" s="145" t="s">
         <v>62</v>
       </c>
@@ -41603,7 +41607,7 @@
       <c r="AI67" s="64"/>
       <c r="AJ67" s="64"/>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A68" s="145" t="s">
         <v>62</v>
       </c>
@@ -41691,7 +41695,7 @@
       <c r="AI68" s="64"/>
       <c r="AJ68" s="64"/>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A69" s="145" t="s">
         <v>62</v>
       </c>
@@ -41779,7 +41783,7 @@
       <c r="AI69" s="64"/>
       <c r="AJ69" s="64"/>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A70" s="145" t="s">
         <v>62</v>
       </c>
@@ -41867,7 +41871,7 @@
       <c r="AI70" s="64"/>
       <c r="AJ70" s="64"/>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A71" s="145" t="s">
         <v>62</v>
       </c>
@@ -41957,14 +41961,20 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="K1:K4"/>
     <mergeCell ref="Q3:Y3"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="O5:P5"/>
@@ -41981,20 +41991,14 @@
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O17:P17"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:J4"/>
-    <mergeCell ref="K1:K4"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>